<commit_message>
restructure for pvp module
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Player.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Player.xlsx
@@ -415,7 +415,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224">
   <si>
     <t>Id</t>
   </si>
@@ -525,6 +525,18 @@
     <t>TeamID</t>
   </si>
   <si>
+    <t>ViewOppnent</t>
+  </si>
+  <si>
+    <t>FightOppnent</t>
+  </si>
+  <si>
+    <t>GambleGold</t>
+  </si>
+  <si>
+    <t>GambleDiamond</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -658,6 +670,12 @@
   </si>
   <si>
     <t>所在队伍ID</t>
+  </si>
+  <si>
+    <t>when searching</t>
+  </si>
+  <si>
+    <t>pvp_oppnent</t>
   </si>
   <si>
     <t>SUCKBLOOD</t>
@@ -1114,10 +1132,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1148,6 +1166,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1156,8 +1181,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1179,7 +1205,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1193,6 +1219,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1201,25 +1234,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1233,15 +1257,32 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1254,31 +1295,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1286,13 +1304,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1313,7 +1331,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1325,31 +1463,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1361,103 +1487,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1469,19 +1505,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1493,7 +1517,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1623,6 +1647,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1630,6 +1669,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1658,17 +1712,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1687,53 +1744,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1743,134 +1767,134 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1966,6 +1990,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2374,12 +2410,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AJ9"/>
+  <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="AO1" sqref="AO$1:AO$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2398,9 +2434,13 @@
     <col min="27" max="27" width="13.6106194690265" customWidth="1"/>
     <col min="30" max="30" width="12.4159292035398" customWidth="1"/>
     <col min="31" max="31" width="15.929203539823" customWidth="1"/>
+    <col min="37" max="37" width="15.6725663716814" customWidth="1"/>
+    <col min="38" max="38" width="14.4778761061947" customWidth="1"/>
+    <col min="39" max="39" width="15.9380530973451" customWidth="1"/>
+    <col min="40" max="40" width="15.929203539823" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="1" spans="1:36">
+    <row r="1" s="27" customFormat="1" spans="1:40">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -2509,120 +2549,144 @@
       <c r="AJ1" s="30" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" s="28" customFormat="1" spans="1:36">
+      <c r="AK1" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" s="28" customFormat="1" spans="1:40">
       <c r="A2" s="31" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" s="28" customFormat="1" spans="1:36">
+        <v>43</v>
+      </c>
+      <c r="AK2" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL2" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM2" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN2" s="32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" s="28" customFormat="1" spans="1:40">
       <c r="A3" s="31" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3" t="b">
         <v>1</v>
@@ -2729,10 +2793,22 @@
       <c r="AJ3" s="3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" s="28" customFormat="1" spans="1:36">
+      <c r="AK3" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="28" customFormat="1" spans="1:40">
       <c r="A4" s="31" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>1</v>
@@ -2839,10 +2915,22 @@
       <c r="AJ4" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" s="28" customFormat="1" spans="1:36">
+      <c r="AK4" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="32" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" s="28" customFormat="1" spans="1:40">
       <c r="A5" s="31" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -2949,10 +3037,22 @@
       <c r="AJ5" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" s="28" customFormat="1" spans="1:36">
+      <c r="AK5" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN5" s="32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" s="28" customFormat="1" spans="1:40">
       <c r="A6" s="31" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -3059,10 +3159,22 @@
       <c r="AJ6" s="3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" s="18" customFormat="1" spans="1:36">
+      <c r="AK6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" s="18" customFormat="1" spans="1:40">
       <c r="A7" s="24" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B7" s="18" t="b">
         <v>0</v>
@@ -3169,10 +3281,22 @@
       <c r="AJ7" s="18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" s="18" customFormat="1" spans="1:36">
+      <c r="AK7" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="18" customFormat="1" spans="1:40">
       <c r="A8" s="24" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B8" s="18" t="b">
         <v>0</v>
@@ -3279,120 +3403,140 @@
       <c r="AJ8" s="18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" s="19" customFormat="1" ht="68.25" spans="1:36">
+      <c r="AK8" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" s="19" customFormat="1" ht="68.25" spans="1:40">
       <c r="A9" s="25" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="N9" s="26" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="O9" s="26" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="Q9" s="26" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="R9" s="26" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="S9" s="26" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="T9" s="26" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="U9" s="26" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="V9" s="26" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="W9" s="26" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="X9" s="26" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="Y9" s="26" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="Z9" s="26" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AA9" s="26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="AB9" s="26" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AC9" s="26" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AD9" s="26" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AE9" s="26" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="AF9" s="26" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AG9" s="26" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AH9" s="26" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AI9" s="26" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AJ9" s="26" t="s">
-        <v>80</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="AK9" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL9" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM9" s="35"/>
+      <c r="AN9" s="35"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3 M3 N3 O3 Q3:T3 U3 V3 W3 X3 Y3 Z3 AA3 AB3 AC3 AD3 AE3 I4 AG7:AJ8 B7:E8 G7:AF8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3 M3 N3 O3 Q3:T3 U3 V3 W3 X3 Y3 Z3 AA3 AB3 AC3 AD3 AE3 I4 AK5 AL5 AK6 AL6 AK7:AK8 AL7:AL8 AM7:AM8 AN7:AN8 AG7:AJ8 B7:E8 G7:AF8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
@@ -3422,188 +3566,188 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="X1" s="21" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="Z1" s="21" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="AA1" s="21" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="AB1" s="21" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="AC1" s="21" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="AD1" s="21" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" s="17" customFormat="1" spans="1:30">
       <c r="A2" s="22" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="N2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="O2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="R2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="S2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="T2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="U2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="V2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="W2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="X2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Y2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Z2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AA2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AB2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AC2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AD2" s="23" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" s="17" customFormat="1" spans="1:30">
       <c r="A3" s="22" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B3" s="23" t="b">
         <v>1</v>
@@ -3695,7 +3839,7 @@
     </row>
     <row r="4" s="17" customFormat="1" spans="1:30">
       <c r="A4" s="22" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B4" s="23" t="b">
         <v>1</v>
@@ -3787,7 +3931,7 @@
     </row>
     <row r="5" s="17" customFormat="1" spans="1:30">
       <c r="A5" s="22" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B5" s="23" t="b">
         <v>0</v>
@@ -3879,7 +4023,7 @@
     </row>
     <row r="6" s="17" customFormat="1" spans="1:30">
       <c r="A6" s="22" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B6" s="23" t="b">
         <v>0</v>
@@ -3971,7 +4115,7 @@
     </row>
     <row r="7" s="18" customFormat="1" spans="1:30">
       <c r="A7" s="24" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B7" s="18" t="b">
         <v>0</v>
@@ -4063,7 +4207,7 @@
     </row>
     <row r="8" s="18" customFormat="1" spans="1:30">
       <c r="A8" s="24" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B8" s="18" t="b">
         <v>0</v>
@@ -4155,94 +4299,94 @@
     </row>
     <row r="9" s="19" customFormat="1" ht="68.25" spans="1:30">
       <c r="A9" s="25" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="N9" s="26" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="O9" s="26" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="Q9" s="26" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="R9" s="26" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="S9" s="26" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="T9" s="26" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="U9" s="26" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="V9" s="26" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="W9" s="26" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="X9" s="26" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="Y9" s="26" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="Z9" s="26" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="AA9" s="26" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="AB9" s="26" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="AC9" s="26" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="AD9" s="26" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -4288,12 +4432,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B2" s="3">
         <v>64</v>
@@ -4301,7 +4445,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B3" s="3">
         <v>22</v>
@@ -4309,7 +4453,7 @@
     </row>
     <row r="4" s="3" customFormat="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>0</v>
@@ -4317,7 +4461,7 @@
     </row>
     <row r="5" s="3" customFormat="1" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -4325,7 +4469,7 @@
     </row>
     <row r="6" s="3" customFormat="1" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -4333,7 +4477,7 @@
     </row>
     <row r="7" s="3" customFormat="1" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -4341,7 +4485,7 @@
     </row>
     <row r="8" s="3" customFormat="1" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -4349,143 +4493,143 @@
     </row>
     <row r="9" s="3" customFormat="1" spans="1:22">
       <c r="A9" s="3" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1" spans="1:22">
       <c r="A10" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B11" s="12"/>
     </row>
@@ -4494,12 +4638,12 @@
         <v>0</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="1" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B13" s="3">
         <v>5</v>
@@ -4507,7 +4651,7 @@
     </row>
     <row r="14" s="3" customFormat="1" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
@@ -4515,7 +4659,7 @@
     </row>
     <row r="15" s="3" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3" t="b">
         <v>0</v>
@@ -4523,7 +4667,7 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B16" s="3" t="b">
         <v>1</v>
@@ -4531,7 +4675,7 @@
     </row>
     <row r="17" s="3" customFormat="1" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B17" s="3" t="b">
         <v>1</v>
@@ -4539,7 +4683,7 @@
     </row>
     <row r="18" s="3" customFormat="1" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3" t="b">
         <v>1</v>
@@ -4547,7 +4691,7 @@
     </row>
     <row r="19" s="3" customFormat="1" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B19" s="3" t="b">
         <v>1</v>
@@ -4555,23 +4699,23 @@
     </row>
     <row r="20" s="3" customFormat="1" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" s="3" customFormat="1" spans="1:2">
       <c r="A21" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B22" s="12"/>
     </row>
@@ -4580,12 +4724,12 @@
         <v>0</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" s="3" customFormat="1" spans="1:2">
       <c r="A24" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B24" s="3">
         <v>15</v>
@@ -4593,7 +4737,7 @@
     </row>
     <row r="25" s="3" customFormat="1" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B25" s="3">
         <v>29</v>
@@ -4601,7 +4745,7 @@
     </row>
     <row r="26" s="3" customFormat="1" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B26" s="3" t="b">
         <v>1</v>
@@ -4609,7 +4753,7 @@
     </row>
     <row r="27" s="3" customFormat="1" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B27" s="3" t="b">
         <v>1</v>
@@ -4617,7 +4761,7 @@
     </row>
     <row r="28" s="3" customFormat="1" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B28" s="3" t="b">
         <v>0</v>
@@ -4625,7 +4769,7 @@
     </row>
     <row r="29" s="3" customFormat="1" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B29" s="3" t="b">
         <v>0</v>
@@ -4633,7 +4777,7 @@
     </row>
     <row r="30" s="3" customFormat="1" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B30" s="3" t="b">
         <v>0</v>
@@ -4641,200 +4785,200 @@
     </row>
     <row r="31" s="3" customFormat="1" spans="1:29">
       <c r="A31" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="U31" s="3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="V31" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="W31" s="3" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="X31" s="3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="Y31" s="3" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="AA31" s="3" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="AB31" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="AC31" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="1" spans="1:29">
       <c r="A32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="U32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="V32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="W32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="X32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Y32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Z32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AA32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AB32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AC32" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" s="3" customFormat="1" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C18 C20:C22 A24:B25 B34:C1048576 A2:B3 A13:B14">
+      <formula1>0</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B8 B18 B19 C33 B29:B30 C23:C29 D33:G1048576 A4:B6 A15:B17 A26:B28 D12:G18 D20:G29">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A32:C32 U32 D31:T32 V31:AC32">
       <formula1>"int,string,float,object"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C18 C20:C22 A24:B25 B34:C1048576 A2:B3 A13:B14">
-      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4875,7 +5019,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -4901,7 +5045,7 @@
     </row>
     <row r="2" s="14" customFormat="1" spans="1:23">
       <c r="A2" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B2" s="3">
         <v>256</v>
@@ -4930,7 +5074,7 @@
     </row>
     <row r="3" s="14" customFormat="1" spans="1:23">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B3" s="3">
         <v>23</v>
@@ -4959,7 +5103,7 @@
     </row>
     <row r="4" s="14" customFormat="1" spans="1:23">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>0</v>
@@ -4988,7 +5132,7 @@
     </row>
     <row r="5" s="14" customFormat="1" spans="1:23">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -5017,7 +5161,7 @@
     </row>
     <row r="6" s="14" customFormat="1" spans="1:23">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -5046,7 +5190,7 @@
     </row>
     <row r="7" s="14" customFormat="1" spans="1:23">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -5075,7 +5219,7 @@
     </row>
     <row r="8" s="14" customFormat="1" spans="1:23">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -5104,152 +5248,152 @@
     </row>
     <row r="9" s="14" customFormat="1" spans="1:23">
       <c r="A9" s="3" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" s="14" customFormat="1" spans="1:23">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" s="14" customFormat="1" spans="1:23">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -5278,7 +5422,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -5304,7 +5448,7 @@
     </row>
     <row r="13" s="15" customFormat="1" spans="1:23">
       <c r="A13" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B13" s="3">
         <v>128</v>
@@ -5333,7 +5477,7 @@
     </row>
     <row r="14" s="15" customFormat="1" spans="1:23">
       <c r="A14" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -5362,7 +5506,7 @@
     </row>
     <row r="15" s="15" customFormat="1" spans="1:23">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3" t="b">
         <v>0</v>
@@ -5391,7 +5535,7 @@
     </row>
     <row r="16" s="15" customFormat="1" spans="1:23">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B16" s="3" t="b">
         <v>1</v>
@@ -5420,7 +5564,7 @@
     </row>
     <row r="17" s="15" customFormat="1" spans="1:23">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B17" s="3" t="b">
         <v>1</v>
@@ -5449,7 +5593,7 @@
     </row>
     <row r="18" s="15" customFormat="1" spans="1:23">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3" t="b">
         <v>1</v>
@@ -5478,7 +5622,7 @@
     </row>
     <row r="19" s="15" customFormat="1" spans="1:23">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B19" s="3" t="b">
         <v>0</v>
@@ -5507,44 +5651,44 @@
     </row>
     <row r="20" s="15" customFormat="1" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
     </row>
     <row r="21" s="15" customFormat="1" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" s="15" customFormat="1" spans="1:23">
       <c r="A22" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -5570,15 +5714,15 @@
     </row>
   </sheetData>
   <dataValidations count="4">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3">
+      <formula1>0</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B8 E11:F11 B18 B19 G11:G19 E1:G8 A4:B6 D22:G1048576 A15:B17 D12:F19">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B9 G9 N9:W9 F9:F10 N1:N8 N11:N19 N22:N1048576"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10 G10 N10:W10 A9:A10 O1:AE8 A20:E21 I11:M19 O11:AE19 I22:M1048576 O22:AE1048576 X9:AE10 C9:E10 H9:M10 I1:M8">
       <formula1>"int,string,float,object"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3">
-      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5632,12 +5776,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B2" s="3">
         <v>15</v>
@@ -5645,7 +5789,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B3" s="3">
         <v>29</v>
@@ -5653,7 +5797,7 @@
     </row>
     <row r="4" s="3" customFormat="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>1</v>
@@ -5661,7 +5805,7 @@
     </row>
     <row r="5" s="3" customFormat="1" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -5669,7 +5813,7 @@
     </row>
     <row r="6" s="3" customFormat="1" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -5677,7 +5821,7 @@
     </row>
     <row r="7" s="3" customFormat="1" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>0</v>
@@ -5685,7 +5829,7 @@
     </row>
     <row r="8" s="3" customFormat="1" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -5693,200 +5837,200 @@
     </row>
     <row r="9" s="3" customFormat="1" spans="1:29">
       <c r="A9" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="AB9" s="3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1" spans="1:29">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 C1:C8 A2:B3 B12:C1048576">
+      <formula1>0</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7:B8 G1:G8 G11:G1048576 D1:F8 D11:F1048576 A4:B5">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:C10 U10 AC1:AC8 AC11:AC1048576 AD$1:AK$1048576 I1:K8 I11:K1048576 L1:AB8 L11:AB1048576 D9:T10 V9:AC10">
       <formula1>"int,string,float,object"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 C1:C8 A2:B3 B12:C1048576">
-      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5923,12 +6067,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" s="6" customFormat="1" spans="1:2">
       <c r="A2" s="9" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B2" s="9">
         <v>8</v>
@@ -5936,7 +6080,7 @@
     </row>
     <row r="3" s="6" customFormat="1" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B3" s="9">
         <v>4</v>
@@ -5944,7 +6088,7 @@
     </row>
     <row r="4" s="6" customFormat="1" spans="1:2">
       <c r="A4" s="9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" s="9" t="b">
         <v>0</v>
@@ -5952,7 +6096,7 @@
     </row>
     <row r="5" s="6" customFormat="1" spans="1:2">
       <c r="A5" s="9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B5" s="9" t="b">
         <v>1</v>
@@ -5960,7 +6104,7 @@
     </row>
     <row r="6" s="6" customFormat="1" spans="1:2">
       <c r="A6" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B6" s="9" t="b">
         <v>1</v>
@@ -5968,7 +6112,7 @@
     </row>
     <row r="7" s="6" customFormat="1" spans="1:2">
       <c r="A7" s="9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -5976,7 +6120,7 @@
     </row>
     <row r="8" s="6" customFormat="1" spans="1:2">
       <c r="A8" s="9" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B8" s="9" t="b">
         <v>0</v>
@@ -5984,38 +6128,38 @@
     </row>
     <row r="9" s="6" customFormat="1" spans="1:4">
       <c r="A9" s="6" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" s="6" customFormat="1" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" s="6" customFormat="1" spans="1:2">
       <c r="A11" s="9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" s="5" customFormat="1" spans="1:2">
@@ -6023,12 +6167,12 @@
         <v>0</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" s="6" customFormat="1" spans="1:2">
       <c r="A13" s="9" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B13" s="9">
         <v>512</v>
@@ -6036,7 +6180,7 @@
     </row>
     <row r="14" s="6" customFormat="1" spans="1:2">
       <c r="A14" s="9" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B14" s="9">
         <v>3</v>
@@ -6044,7 +6188,7 @@
     </row>
     <row r="15" s="6" customFormat="1" spans="1:2">
       <c r="A15" s="9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B15" s="9" t="b">
         <v>0</v>
@@ -6052,7 +6196,7 @@
     </row>
     <row r="16" s="6" customFormat="1" spans="1:2">
       <c r="A16" s="9" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B16" s="9" t="b">
         <v>1</v>
@@ -6060,7 +6204,7 @@
     </row>
     <row r="17" s="6" customFormat="1" spans="1:2">
       <c r="A17" s="9" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B17" s="9" t="b">
         <v>1</v>
@@ -6068,7 +6212,7 @@
     </row>
     <row r="18" s="6" customFormat="1" spans="1:2">
       <c r="A18" s="9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3" t="b">
         <v>1</v>
@@ -6076,7 +6220,7 @@
     </row>
     <row r="19" s="6" customFormat="1" spans="1:2">
       <c r="A19" s="9" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B19" s="9" t="b">
         <v>0</v>
@@ -6084,47 +6228,47 @@
     </row>
     <row r="20" s="6" customFormat="1" spans="1:3">
       <c r="A20" s="6" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
     </row>
     <row r="21" s="6" customFormat="1" spans="1:3">
       <c r="A21" s="6" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" s="6" customFormat="1" spans="1:2">
       <c r="A22" s="9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A9:D10 I$1:L$1048576 A20:B21">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3">
+      <formula1>0</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B8 B18 G1:G21 A4:B6 A15:B17 E1:F11 D12:F21 D22:G1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
       <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A9:D10 I$1:L$1048576 A20:B21">
-      <formula1>"int,float,string,object"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6163,12 +6307,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B2" s="3">
         <v>128</v>
@@ -6176,7 +6320,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B3" s="3">
         <v>8</v>
@@ -6184,7 +6328,7 @@
     </row>
     <row r="4" s="3" customFormat="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>0</v>
@@ -6192,7 +6336,7 @@
     </row>
     <row r="5" s="3" customFormat="1" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -6200,7 +6344,7 @@
     </row>
     <row r="6" s="3" customFormat="1" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -6208,7 +6352,7 @@
     </row>
     <row r="7" s="3" customFormat="1" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -6216,7 +6360,7 @@
     </row>
     <row r="8" s="3" customFormat="1" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -6224,59 +6368,59 @@
     </row>
     <row r="9" s="3" customFormat="1" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:1">
       <c r="A11" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" spans="1:2">
@@ -6284,12 +6428,12 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>212</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="1" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B13" s="3">
         <v>128</v>
@@ -6297,7 +6441,7 @@
     </row>
     <row r="14" s="3" customFormat="1" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="B14" s="3">
         <v>8</v>
@@ -6305,7 +6449,7 @@
     </row>
     <row r="15" s="3" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B15" s="3" t="b">
         <v>0</v>
@@ -6313,7 +6457,7 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B16" s="3" t="b">
         <v>1</v>
@@ -6321,7 +6465,7 @@
     </row>
     <row r="17" s="3" customFormat="1" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B17" s="3" t="b">
         <v>1</v>
@@ -6329,7 +6473,7 @@
     </row>
     <row r="18" s="3" customFormat="1" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3" t="b">
         <v>1</v>
@@ -6337,7 +6481,7 @@
     </row>
     <row r="19" s="3" customFormat="1" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B19" s="3" t="b">
         <v>0</v>
@@ -6345,77 +6489,77 @@
     </row>
     <row r="20" s="3" customFormat="1" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" s="3" customFormat="1" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:1">
       <c r="A22" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="6">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A2:B3 A13:B14">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:B10 D10:F10 A21:B21 D21:F21 K1:K39">
+      <formula1>"int,float,string,object"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B8 E11:F11 B18 B19 I$1:I$1048576 G11:H19 D22:H1048576 A4:B6 A15:B17 E1:H8 D12:F19">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A9:B9 D9:F9 A20:B20 D20:F20 K40:K1048576"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8 A18:A19"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:B10 D10:F10 A21:B21 D21:F21 K1:K39">
-      <formula1>"int,float,string,object"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C21">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A2:B3 A13:B14">
-      <formula1>0</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8 A18:A19"/>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -6444,27 +6588,27 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C1" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allocate memory for record when load data for it from database
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Player.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="10342"/>
+    <workbookView windowWidth="21495" windowHeight="10342" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -1132,10 +1132,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -1160,30 +1160,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1198,16 +1182,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1219,8 +1203,92 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1234,77 +1302,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1337,25 +1337,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1367,7 +1379,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1379,7 +1391,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1391,25 +1403,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1427,7 +1421,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1439,85 +1499,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1647,6 +1647,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1658,41 +1667,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1715,8 +1689,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1724,8 +1698,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1744,153 +1718,179 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2412,10 +2412,10 @@
   <sheetPr/>
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AO1" sqref="AO$1:AO$1048576"/>
+      <selection pane="bottomLeft" activeCell="AM6" sqref="AM6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2932,110 +2932,110 @@
       <c r="A5" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="N5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="O5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="T5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="U5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="V5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="W5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="X5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AD5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AG5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AH5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI5" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AJ5" s="3" t="b">
-        <v>1</v>
+      <c r="B5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="M5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="O5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="T5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="U5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="V5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="W5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="X5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="18" t="b">
+        <v>0</v>
       </c>
       <c r="AK5" s="33" t="b">
         <v>0</v>
@@ -3044,10 +3044,10 @@
         <v>0</v>
       </c>
       <c r="AM5" s="32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN5" s="32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" s="28" customFormat="1" spans="1:40">
@@ -3166,10 +3166,10 @@
         <v>0</v>
       </c>
       <c r="AM6" s="32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN6" s="32" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" s="18" customFormat="1" spans="1:40">
@@ -3536,7 +3536,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3 M3 N3 O3 Q3:T3 U3 V3 W3 X3 Y3 Z3 AA3 AB3 AC3 AD3 AE3 I4 AK5 AL5 AK6 AL6 AK7:AK8 AL7:AL8 AM7:AM8 AN7:AN8 AG7:AJ8 B7:E8 G7:AF8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3 M3 N3 O3 Q3:T3 U3 V3 W3 X3 Y3 Z3 AA3 AB3 AC3 AD3 AE3 I4 B5:AJ5 AK5 AL5 AK6 AL6 AK7:AK8 AL7:AL8 AM7:AM8 AN7:AN8 AG7:AJ8 B7:E8 G7:AF8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
@@ -4408,7 +4408,7 @@
   <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4472,7 +4472,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:2">
@@ -4678,7 +4678,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" s="3" customFormat="1" spans="1:2">
@@ -4971,14 +4971,14 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C18 C20:C22 A24:B25 B34:C1048576 A2:B3 A13:B14">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B8 B18 B19 C33 B29:B30 C23:C29 D33:G1048576 A4:B6 A15:B17 A26:B28 D12:G18 D20:G29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 A17 B17 B18 B19 A28 B28 C33 B29:B30 C23:C29 D33:G1048576 D12:G18 D20:G29 A4:B5 A15:B16 A26:B27">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A32:C32 U32 D31:T32 V31:AC32">
       <formula1>"int,string,float,object"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C18 C20:C22 A24:B25 B34:C1048576 A2:B3 A13:B14">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5164,7 +5164,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -5567,7 +5567,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -5714,15 +5714,15 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B8 E11:F11 B18 B19 G11:G19 E1:G8 A4:B6 D22:G1048576 A15:B17 D12:F19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 E11:F11 A17 B17 B18 B19 G11:G19 E1:G8 D22:G1048576 D12:F19 A15:B16 A4:B5">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B9 G9 N9:W9 F9:F10 N1:N8 N11:N19 N22:N1048576"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10 G10 N10:W10 A9:A10 O1:AE8 A20:E21 I11:M19 O11:AE19 I22:M1048576 O22:AE1048576 X9:AE10 C9:E10 H9:M10 I1:M8">
       <formula1>"int,string,float,object"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5816,7 +5816,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:2">
@@ -6023,14 +6023,14 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 C1:C8 A2:B3 B12:C1048576">
-      <formula1>0</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7:B8 G1:G8 G11:G1048576 D1:F8 D11:F1048576 A4:B5">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:C10 U10 AC1:AC8 AC11:AC1048576 AD$1:AK$1048576 I1:K8 I11:K1048576 L1:AB8 L11:AB1048576 D9:T10 V9:AC10">
       <formula1>"int,string,float,object"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 C1:C8 A2:B3 B12:C1048576">
+      <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6046,7 +6046,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -6107,7 +6107,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" s="6" customFormat="1" spans="1:2">
@@ -6207,7 +6207,7 @@
         <v>46</v>
       </c>
       <c r="B17" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" s="6" customFormat="1" spans="1:2">
@@ -6258,17 +6258,17 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A9:D10 I$1:L$1048576 A20:B21">
-      <formula1>"int,float,string,object"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 A17 B17 B18 G1:G21 E1:F11 D12:F21 D22:G1048576 A4:B5 A15:B16">
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B8 B18 G1:G21 A4:B6 A15:B17 E1:F11 D12:F21 D22:G1048576">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
-      <formula1>"true,false"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A9:D10 I$1:L$1048576 A20:B21">
+      <formula1>"int,float,string,object"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6283,8 +6283,8 @@
   <sheetPr/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -6347,7 +6347,7 @@
         <v>46</v>
       </c>
       <c r="B6" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" s="3" customFormat="1" spans="1:2">
@@ -6546,20 +6546,20 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A2:B3 A13:B14">
-      <formula1>0</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 E11:F11 B18 B19 I$1:I$1048576 G11:H19 D22:H1048576 A15:B17 E1:H8 D12:F19 A4:B5">
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A9:B9 D9:F9 A20:B20 D20:F20 K40:K1048576"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:B10 D10:F10 A21:B21 D21:F21 K1:K39">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B8 E11:F11 B18 B19 I$1:I$1048576 G11:H19 D22:H1048576 A4:B6 A15:B17 E1:H8 D12:F19">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A9:B9 D9:F9 A20:B20 D20:F20 K40:K1048576"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C21">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8 A18:A19"/>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A2:B3 A13:B14">
+      <formula1>0</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
add security plugin add aoi plugin add hero switch function remove unused files
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Player.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="10342" firstSheet="1" activeTab="6"/>
+    <workbookView windowWidth="21495" windowHeight="10342"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -537,6 +537,9 @@
     <t>GambleDiamond</t>
   </si>
   <si>
+    <t>FightHero</t>
+  </si>
+  <si>
     <t>Type</t>
   </si>
   <si>
@@ -916,9 +919,6 @@
   </si>
   <si>
     <t>PlayerFightHero</t>
-  </si>
-  <si>
-    <t>FightPos</t>
   </si>
   <si>
     <t>HeroPropertyValue</t>
@@ -1160,7 +1160,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1168,6 +1175,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1181,23 +1195,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1211,20 +1242,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -1233,16 +1250,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1256,8 +1273,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1270,33 +1295,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1337,31 +1337,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1379,7 +1427,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1391,37 +1469,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1439,85 +1511,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1656,6 +1656,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1671,16 +1686,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1697,24 +1712,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1736,11 +1738,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1749,152 +1749,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1982,14 +1982,20 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2410,17 +2416,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AN9"/>
+  <dimension ref="A1:AO9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="AM6" sqref="AM6"/>
+      <selection pane="bottomLeft" activeCell="AO1" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="23.8141592920354" customWidth="1"/>
+    <col min="1" max="1" width="23.8141592920354" style="29" customWidth="1"/>
     <col min="2" max="2" width="8.17699115044248" customWidth="1"/>
     <col min="3" max="3" width="10.4513274336283" customWidth="1"/>
     <col min="4" max="4" width="11.6371681415929" customWidth="1"/>
@@ -2438,115 +2444,116 @@
     <col min="38" max="38" width="14.4778761061947" customWidth="1"/>
     <col min="39" max="39" width="15.9380530973451" customWidth="1"/>
     <col min="40" max="40" width="15.929203539823" customWidth="1"/>
+    <col min="41" max="41" width="11.2212389380531" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="27" customFormat="1" spans="1:40">
-      <c r="A1" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="30" t="s">
+    <row r="1" s="27" customFormat="1" spans="1:41">
+      <c r="A1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="K1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="M1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="30" t="s">
+      <c r="Q1" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="R1" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="30" t="s">
+      <c r="S1" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="30" t="s">
+      <c r="T1" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="30" t="s">
+      <c r="U1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="30" t="s">
+      <c r="V1" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="30" t="s">
+      <c r="W1" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="30" t="s">
+      <c r="X1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="30" t="s">
+      <c r="Y1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="30" t="s">
+      <c r="Z1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="30" t="s">
+      <c r="AA1" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="30" t="s">
+      <c r="AB1" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="30" t="s">
+      <c r="AC1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="30" t="s">
+      <c r="AD1" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="30" t="s">
+      <c r="AE1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="30" t="s">
+      <c r="AF1" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="30" t="s">
+      <c r="AG1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="30" t="s">
+      <c r="AH1" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="30" t="s">
+      <c r="AI1" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="30" t="s">
+      <c r="AJ1" s="31" t="s">
         <v>35</v>
       </c>
       <c r="AK1" s="27" t="s">
@@ -2561,133 +2568,139 @@
       <c r="AN1" s="27" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" s="28" customFormat="1" spans="1:40">
-      <c r="A2" s="31" t="s">
+      <c r="AO1" s="27" t="s">
         <v>40</v>
       </c>
+    </row>
+    <row r="2" s="28" customFormat="1" spans="1:41">
+      <c r="A2" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="J2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="W2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AD2" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AG2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AJ2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK2" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL2" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="AM2" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN2" s="32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" s="28" customFormat="1" spans="1:40">
-      <c r="A3" s="31" t="s">
         <v>44</v>
       </c>
+      <c r="AK2" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL2" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM2" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN2" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" s="28" customFormat="1" spans="1:41">
+      <c r="A3" s="32" t="s">
+        <v>45</v>
+      </c>
       <c r="B3" s="3" t="b">
         <v>1</v>
       </c>
@@ -2793,22 +2806,25 @@
       <c r="AJ3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="AK3" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" s="28" customFormat="1" spans="1:40">
-      <c r="A4" s="31" t="s">
-        <v>45</v>
+      <c r="AK3" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="28" customFormat="1" spans="1:41">
+      <c r="A4" s="32" t="s">
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>1</v>
@@ -2915,22 +2931,25 @@
       <c r="AJ4" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AK4" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN4" s="32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" s="28" customFormat="1" spans="1:40">
-      <c r="A5" s="31" t="s">
-        <v>46</v>
+      <c r="AK4" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" s="28" customFormat="1" spans="1:41">
+      <c r="A5" s="32" t="s">
+        <v>47</v>
       </c>
       <c r="B5" s="18" t="b">
         <v>0</v>
@@ -3037,22 +3056,25 @@
       <c r="AJ5" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="AK5" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" s="28" customFormat="1" spans="1:40">
-      <c r="A6" s="31" t="s">
-        <v>47</v>
+      <c r="AK5" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="28" customFormat="1" spans="1:41">
+      <c r="A6" s="32" t="s">
+        <v>48</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>1</v>
@@ -3159,22 +3181,25 @@
       <c r="AJ6" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AK6" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="32" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="18" customFormat="1" spans="1:40">
-      <c r="A7" s="24" t="s">
-        <v>48</v>
+      <c r="AK6" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" s="18" customFormat="1" spans="1:41">
+      <c r="A7" s="33" t="s">
+        <v>49</v>
       </c>
       <c r="B7" s="18" t="b">
         <v>0</v>
@@ -3281,22 +3306,25 @@
       <c r="AJ7" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="AK7" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" s="18" customFormat="1" spans="1:40">
-      <c r="A8" s="24" t="s">
-        <v>49</v>
+      <c r="AK7" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="18" customFormat="1" spans="1:41">
+      <c r="A8" s="33" t="s">
+        <v>50</v>
       </c>
       <c r="B8" s="18" t="b">
         <v>0</v>
@@ -3403,143 +3431,146 @@
       <c r="AJ8" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="AK8" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AM8" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="33" t="b">
+      <c r="AK8" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="35" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="18" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" s="19" customFormat="1" ht="68.25" spans="1:40">
       <c r="A9" s="25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H9" s="26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N9" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="O9" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="26" t="s">
-        <v>62</v>
-      </c>
       <c r="P9" s="26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Q9" s="26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R9" s="26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S9" s="26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="T9" s="26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="U9" s="26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="V9" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="W9" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="X9" s="26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y9" s="26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Z9" s="26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="AA9" s="26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AB9" s="26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AC9" s="26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AD9" s="26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AE9" s="26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="AF9" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AG9" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AH9" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AI9" s="26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AJ9" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK9" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="AL9" s="34" t="s">
+      <c r="AK9" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="AM9" s="35"/>
-      <c r="AN9" s="35"/>
+      <c r="AL9" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="AM9" s="37"/>
+      <c r="AN9" s="37"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3 M3 N3 O3 Q3:T3 U3 V3 W3 X3 Y3 Z3 AA3 AB3 AC3 AD3 AE3 I4 B5:AJ5 AK5 AL5 AK6 AL6 AK7:AK8 AL7:AL8 AM7:AM8 AN7:AN8 AG7:AJ8 B7:E8 G7:AF8">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3 M3 N3 O3 Q3:T3 U3 V3 W3 X3 Y3 Z3 AA3 AB3 AC3 AD3 AE3 I4 B5:AJ5 AK5 AL5 AO5 AK6 AL6 AK7:AK8 AL7:AL8 AM7:AM8 AN7:AN8 AO7:AO8 AG7:AJ8 B7:E8 G7:AF8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -3566,188 +3597,188 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H1" s="21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="I1" s="21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L1" s="21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M1" s="21" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="P1" s="21" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="T1" s="21" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="U1" s="21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V1" s="21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="W1" s="21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="X1" s="21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Y1" s="21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Z1" s="21" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AA1" s="21" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AB1" s="21" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AC1" s="21" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AD1" s="21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" s="17" customFormat="1" spans="1:30">
       <c r="A2" s="22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AA2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AD2" s="23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" s="17" customFormat="1" spans="1:30">
       <c r="A3" s="22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" s="23" t="b">
         <v>1</v>
@@ -3839,7 +3870,7 @@
     </row>
     <row r="4" s="17" customFormat="1" spans="1:30">
       <c r="A4" s="22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B4" s="23" t="b">
         <v>1</v>
@@ -3931,7 +3962,7 @@
     </row>
     <row r="5" s="17" customFormat="1" spans="1:30">
       <c r="A5" s="22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B5" s="23" t="b">
         <v>0</v>
@@ -4023,7 +4054,7 @@
     </row>
     <row r="6" s="17" customFormat="1" spans="1:30">
       <c r="A6" s="22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B6" s="23" t="b">
         <v>0</v>
@@ -4115,7 +4146,7 @@
     </row>
     <row r="7" s="18" customFormat="1" spans="1:30">
       <c r="A7" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B7" s="18" t="b">
         <v>0</v>
@@ -4207,7 +4238,7 @@
     </row>
     <row r="8" s="18" customFormat="1" spans="1:30">
       <c r="A8" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" s="18" t="b">
         <v>0</v>
@@ -4299,102 +4330,102 @@
     </row>
     <row r="9" s="19" customFormat="1" ht="68.25" spans="1:30">
       <c r="A9" s="25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F9" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="26" t="s">
-        <v>65</v>
-      </c>
       <c r="H9" s="26" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J9" s="26" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="L9" s="26" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="M9" s="26" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="N9" s="26" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="O9" s="26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="P9" s="26" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="Q9" s="26" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="R9" s="26" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="S9" s="26" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="T9" s="26" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="U9" s="26" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="V9" s="26" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="W9" s="26" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="X9" s="26" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Y9" s="26" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="Z9" s="26" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA9" s="26" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AB9" s="26" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AC9" s="26" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AD9" s="26" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7 A8"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:I7 J7:AD7 B8:AD8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7 A8"/>
   </dataValidations>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -4408,7 +4439,7 @@
   <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4432,12 +4463,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B2" s="3">
         <v>64</v>
@@ -4445,7 +4476,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" s="3">
         <v>22</v>
@@ -4453,7 +4484,7 @@
     </row>
     <row r="4" s="3" customFormat="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>0</v>
@@ -4461,7 +4492,7 @@
     </row>
     <row r="5" s="3" customFormat="1" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -4469,7 +4500,7 @@
     </row>
     <row r="6" s="3" customFormat="1" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>0</v>
@@ -4477,7 +4508,7 @@
     </row>
     <row r="7" s="3" customFormat="1" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -4485,7 +4516,7 @@
     </row>
     <row r="8" s="3" customFormat="1" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -4493,143 +4524,143 @@
     </row>
     <row r="9" s="3" customFormat="1" spans="1:22">
       <c r="A9" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1" spans="1:22">
       <c r="A10" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="M10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="N10" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="O10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="12"/>
     </row>
@@ -4638,28 +4669,28 @@
         <v>0</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" s="3" customFormat="1" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B13" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" s="3" customFormat="1" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B14" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="3" t="b">
         <v>0</v>
@@ -4667,7 +4698,7 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3" t="b">
         <v>1</v>
@@ -4675,7 +4706,7 @@
     </row>
     <row r="17" s="3" customFormat="1" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="b">
         <v>0</v>
@@ -4683,7 +4714,7 @@
     </row>
     <row r="18" s="3" customFormat="1" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="b">
         <v>1</v>
@@ -4691,31 +4722,25 @@
     </row>
     <row r="19" s="3" customFormat="1" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="20" s="3" customFormat="1" spans="1:2">
+    <row r="20" s="3" customFormat="1" spans="1:1">
       <c r="A20" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" s="3" customFormat="1" spans="1:2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" s="3" customFormat="1" spans="1:1">
       <c r="A21" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="12"/>
     </row>
@@ -4729,7 +4754,7 @@
     </row>
     <row r="24" s="3" customFormat="1" spans="1:2">
       <c r="A24" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B24" s="3">
         <v>15</v>
@@ -4737,7 +4762,7 @@
     </row>
     <row r="25" s="3" customFormat="1" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B25" s="3">
         <v>29</v>
@@ -4745,7 +4770,7 @@
     </row>
     <row r="26" s="3" customFormat="1" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B26" s="3" t="b">
         <v>1</v>
@@ -4753,7 +4778,7 @@
     </row>
     <row r="27" s="3" customFormat="1" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B27" s="3" t="b">
         <v>1</v>
@@ -4761,7 +4786,7 @@
     </row>
     <row r="28" s="3" customFormat="1" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B28" s="3" t="b">
         <v>0</v>
@@ -4769,7 +4794,7 @@
     </row>
     <row r="29" s="3" customFormat="1" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B29" s="3" t="b">
         <v>0</v>
@@ -4777,7 +4802,7 @@
     </row>
     <row r="30" s="3" customFormat="1" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B30" s="3" t="b">
         <v>0</v>
@@ -4785,185 +4810,185 @@
     </row>
     <row r="31" s="3" customFormat="1" spans="1:29">
       <c r="A31" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N31" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P31" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="R31" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T31" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U31" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V31" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="W31" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="X31" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Y31" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AA31" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AB31" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AC31" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" s="3" customFormat="1" spans="1:29">
       <c r="A32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AA32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC32" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" s="3" customFormat="1" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>169</v>
@@ -5045,7 +5070,7 @@
     </row>
     <row r="2" s="14" customFormat="1" spans="1:23">
       <c r="A2" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B2" s="3">
         <v>256</v>
@@ -5074,7 +5099,7 @@
     </row>
     <row r="3" s="14" customFormat="1" spans="1:23">
       <c r="A3" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" s="3">
         <v>23</v>
@@ -5103,7 +5128,7 @@
     </row>
     <row r="4" s="14" customFormat="1" spans="1:23">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>0</v>
@@ -5132,7 +5157,7 @@
     </row>
     <row r="5" s="14" customFormat="1" spans="1:23">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -5161,7 +5186,7 @@
     </row>
     <row r="6" s="14" customFormat="1" spans="1:23">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>0</v>
@@ -5190,7 +5215,7 @@
     </row>
     <row r="7" s="14" customFormat="1" spans="1:23">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -5219,7 +5244,7 @@
     </row>
     <row r="8" s="14" customFormat="1" spans="1:23">
       <c r="A8" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="b">
         <v>0</v>
@@ -5248,13 +5273,13 @@
     </row>
     <row r="9" s="14" customFormat="1" spans="1:23">
       <c r="A9" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>171</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>172</v>
@@ -5319,78 +5344,78 @@
     </row>
     <row r="10" s="14" customFormat="1" spans="1:23">
       <c r="A10" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="G10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="J10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" s="14" customFormat="1" spans="1:23">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>192</v>
@@ -5448,7 +5473,7 @@
     </row>
     <row r="13" s="15" customFormat="1" spans="1:23">
       <c r="A13" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B13" s="3">
         <v>128</v>
@@ -5477,7 +5502,7 @@
     </row>
     <row r="14" s="15" customFormat="1" spans="1:23">
       <c r="A14" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -5506,7 +5531,7 @@
     </row>
     <row r="15" s="15" customFormat="1" spans="1:23">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="3" t="b">
         <v>0</v>
@@ -5535,7 +5560,7 @@
     </row>
     <row r="16" s="15" customFormat="1" spans="1:23">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3" t="b">
         <v>1</v>
@@ -5564,7 +5589,7 @@
     </row>
     <row r="17" s="15" customFormat="1" spans="1:23">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="b">
         <v>0</v>
@@ -5593,7 +5618,7 @@
     </row>
     <row r="18" s="15" customFormat="1" spans="1:23">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="b">
         <v>1</v>
@@ -5622,7 +5647,7 @@
     </row>
     <row r="19" s="15" customFormat="1" spans="1:23">
       <c r="A19" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="3" t="b">
         <v>0</v>
@@ -5651,7 +5676,7 @@
     </row>
     <row r="20" s="15" customFormat="1" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>194</v>
@@ -5668,24 +5693,24 @@
     </row>
     <row r="21" s="15" customFormat="1" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" s="15" customFormat="1" spans="1:23">
       <c r="A22" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>192</v>
@@ -5717,10 +5742,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 E11:F11 A17 B17 B18 B19 G11:G19 E1:G8 D22:G1048576 D12:F19 A15:B16 A4:B5">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B9 G9 N9:W9 F9:F10 N1:N8 N11:N19 N22:N1048576"/>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10 G10 N10:W10 A9:A10 O1:AE8 A20:E21 I11:M19 O11:AE19 I22:M1048576 O22:AE1048576 X9:AE10 C9:E10 H9:M10 I1:M8">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B9 G9 N9:W9 F9:F10 N1:N8 N11:N19 N22:N1048576"/>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3">
       <formula1>0</formula1>
     </dataValidation>
@@ -5781,7 +5806,7 @@
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B2" s="3">
         <v>15</v>
@@ -5789,7 +5814,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" s="3">
         <v>29</v>
@@ -5797,7 +5822,7 @@
     </row>
     <row r="4" s="3" customFormat="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>1</v>
@@ -5805,7 +5830,7 @@
     </row>
     <row r="5" s="3" customFormat="1" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -5813,7 +5838,7 @@
     </row>
     <row r="6" s="3" customFormat="1" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>0</v>
@@ -5821,7 +5846,7 @@
     </row>
     <row r="7" s="3" customFormat="1" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>0</v>
@@ -5837,185 +5862,185 @@
     </row>
     <row r="9" s="3" customFormat="1" spans="1:29">
       <c r="A9" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AA9" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AB9" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" s="3" customFormat="1" spans="1:29">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AA10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>169</v>
@@ -6046,7 +6071,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -6072,7 +6097,7 @@
     </row>
     <row r="2" s="6" customFormat="1" spans="1:2">
       <c r="A2" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B2" s="9">
         <v>8</v>
@@ -6080,7 +6105,7 @@
     </row>
     <row r="3" s="6" customFormat="1" spans="1:2">
       <c r="A3" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" s="9">
         <v>4</v>
@@ -6088,7 +6113,7 @@
     </row>
     <row r="4" s="6" customFormat="1" spans="1:2">
       <c r="A4" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="9" t="b">
         <v>0</v>
@@ -6096,7 +6121,7 @@
     </row>
     <row r="5" s="6" customFormat="1" spans="1:2">
       <c r="A5" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="9" t="b">
         <v>1</v>
@@ -6104,7 +6129,7 @@
     </row>
     <row r="6" s="6" customFormat="1" spans="1:2">
       <c r="A6" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="9" t="b">
         <v>0</v>
@@ -6112,7 +6137,7 @@
     </row>
     <row r="7" s="6" customFormat="1" spans="1:2">
       <c r="A7" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -6142,21 +6167,21 @@
     </row>
     <row r="10" s="6" customFormat="1" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" s="6" customFormat="1" spans="1:2">
       <c r="A11" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>204</v>
@@ -6172,7 +6197,7 @@
     </row>
     <row r="13" s="6" customFormat="1" spans="1:2">
       <c r="A13" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B13" s="9">
         <v>512</v>
@@ -6180,7 +6205,7 @@
     </row>
     <row r="14" s="6" customFormat="1" spans="1:2">
       <c r="A14" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B14" s="9">
         <v>3</v>
@@ -6188,7 +6213,7 @@
     </row>
     <row r="15" s="6" customFormat="1" spans="1:2">
       <c r="A15" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="9" t="b">
         <v>0</v>
@@ -6196,7 +6221,7 @@
     </row>
     <row r="16" s="6" customFormat="1" spans="1:2">
       <c r="A16" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="9" t="b">
         <v>1</v>
@@ -6204,7 +6229,7 @@
     </row>
     <row r="17" s="6" customFormat="1" spans="1:2">
       <c r="A17" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="9" t="b">
         <v>0</v>
@@ -6212,7 +6237,7 @@
     </row>
     <row r="18" s="6" customFormat="1" spans="1:2">
       <c r="A18" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="b">
         <v>1</v>
@@ -6239,18 +6264,18 @@
     </row>
     <row r="21" s="6" customFormat="1" spans="1:3">
       <c r="A21" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" s="6" customFormat="1" spans="1:2">
       <c r="A22" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>208</v>
@@ -6258,11 +6283,11 @@
     </row>
   </sheetData>
   <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 A17 B17 B18 G1:G21 E1:F11 D12:F21 D22:G1048576 A4:B5 A15:B16">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
       <formula1>"true,false"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 A17 B17 B18 G1:G21 E1:F11 D12:F21 D22:G1048576 A4:B5 A15:B16">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3">
       <formula1>0</formula1>
@@ -6283,8 +6308,8 @@
   <sheetPr/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
@@ -6312,7 +6337,7 @@
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B2" s="3">
         <v>128</v>
@@ -6320,7 +6345,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" s="3">
         <v>8</v>
@@ -6328,7 +6353,7 @@
     </row>
     <row r="4" s="3" customFormat="1" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3" t="b">
         <v>0</v>
@@ -6336,7 +6361,7 @@
     </row>
     <row r="5" s="3" customFormat="1" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3" t="b">
         <v>1</v>
@@ -6344,7 +6369,7 @@
     </row>
     <row r="6" s="3" customFormat="1" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="b">
         <v>0</v>
@@ -6352,7 +6377,7 @@
     </row>
     <row r="7" s="3" customFormat="1" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B7" s="3" t="b">
         <v>1</v>
@@ -6394,33 +6419,33 @@
     </row>
     <row r="10" s="3" customFormat="1" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" s="3" customFormat="1" spans="1:1">
       <c r="A11" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" spans="1:2">
@@ -6433,7 +6458,7 @@
     </row>
     <row r="13" s="3" customFormat="1" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B13" s="3">
         <v>128</v>
@@ -6441,7 +6466,7 @@
     </row>
     <row r="14" s="3" customFormat="1" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B14" s="3">
         <v>8</v>
@@ -6449,7 +6474,7 @@
     </row>
     <row r="15" s="3" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="3" t="b">
         <v>0</v>
@@ -6457,7 +6482,7 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3" t="b">
         <v>1</v>
@@ -6465,7 +6490,7 @@
     </row>
     <row r="17" s="3" customFormat="1" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B17" s="3" t="b">
         <v>1</v>
@@ -6473,7 +6498,7 @@
     </row>
     <row r="18" s="3" customFormat="1" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="b">
         <v>1</v>
@@ -6481,7 +6506,7 @@
     </row>
     <row r="19" s="3" customFormat="1" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B19" s="3" t="b">
         <v>0</v>
@@ -6515,37 +6540,38 @@
     </row>
     <row r="21" s="3" customFormat="1" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" s="3" customFormat="1" spans="1:1">
       <c r="A22" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8 A18:A19"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 E11:F11 B18 B19 I$1:I$1048576 G11:H19 D22:H1048576 A15:B17 E1:H8 D12:F19 A4:B5">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
@@ -6556,7 +6582,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C21">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8 A18:A19"/>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A2:B3 A13:B14">
       <formula1>0</formula1>
     </dataValidation>
@@ -6594,7 +6619,7 @@
         <v>220</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>

<commit_message>
skill property for each hero
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Player.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Player.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -420,7 +420,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="230">
   <si>
     <t>Id</t>
   </si>
@@ -1843,11 +1843,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ9"/>
+  <dimension ref="A1:AT9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1861,19 +1861,19 @@
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="14" width="17.33203125" customWidth="1"/>
-    <col min="24" max="24" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.59765625" customWidth="1"/>
-    <col min="30" max="30" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.3984375" customWidth="1"/>
-    <col min="33" max="33" width="15.9296875" customWidth="1"/>
-    <col min="39" max="39" width="18.33203125" customWidth="1"/>
-    <col min="40" max="40" width="15.6640625" customWidth="1"/>
-    <col min="41" max="41" width="14.46484375" customWidth="1"/>
-    <col min="42" max="43" width="15.9296875" customWidth="1"/>
+    <col min="11" max="17" width="17.33203125" customWidth="1"/>
+    <col min="27" max="27" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.59765625" customWidth="1"/>
+    <col min="33" max="33" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.3984375" customWidth="1"/>
+    <col min="36" max="36" width="15.9296875" customWidth="1"/>
+    <col min="42" max="42" width="18.33203125" customWidth="1"/>
+    <col min="43" max="43" width="15.6640625" customWidth="1"/>
+    <col min="44" max="44" width="14.46484375" customWidth="1"/>
+    <col min="45" max="46" width="15.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="25" customFormat="1">
+    <row r="1" spans="1:46" s="25" customFormat="1">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -1917,94 +1917,103 @@
         <v>225</v>
       </c>
       <c r="O1" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="R1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="S1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="V1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="X1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="Y1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="Z1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="AA1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="28" t="s">
+      <c r="AB1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AC1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AD1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AE1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="28" t="s">
+      <c r="AF1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="28" t="s">
+      <c r="AG1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="28" t="s">
+      <c r="AH1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AF1" s="28" t="s">
+      <c r="AI1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" s="28" t="s">
+      <c r="AJ1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="AH1" s="28" t="s">
+      <c r="AK1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="28" t="s">
+      <c r="AL1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="AJ1" s="28" t="s">
+      <c r="AM1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="28" t="s">
+      <c r="AN1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AL1" s="28" t="s">
+      <c r="AO1" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="AM1" s="28" t="s">
+      <c r="AP1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="AN1" s="25" t="s">
+      <c r="AQ1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" s="25" t="s">
+      <c r="AR1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" s="25" t="s">
+      <c r="AS1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" s="25" t="s">
+      <c r="AT1" s="25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:43" s="26" customFormat="1">
+    <row r="2" spans="1:46" s="26" customFormat="1">
       <c r="A2" s="29" t="s">
         <v>39</v>
       </c>
@@ -2047,14 +2056,14 @@
       <c r="N2" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>41</v>
+      <c r="O2" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q2" s="39" t="s">
+        <v>40</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>41</v>
@@ -2072,20 +2081,20 @@
         <v>41</v>
       </c>
       <c r="W2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="Y2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="AB2" s="3" t="s">
         <v>41</v>
       </c>
@@ -2096,46 +2105,55 @@
         <v>41</v>
       </c>
       <c r="AE2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AH2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="AK2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AM2" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN2" s="30" t="s">
+      <c r="AP2" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AO2" s="30" t="s">
+      <c r="AR2" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AP2" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ2" s="30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" s="26" customFormat="1">
+      <c r="AS2" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="AT2" s="30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" s="26" customFormat="1">
       <c r="A3" s="29" t="s">
         <v>43</v>
       </c>
@@ -2178,17 +2196,17 @@
       <c r="N3" s="39" t="b">
         <v>0</v>
       </c>
-      <c r="O3" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="P3" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="R3" s="3" t="b">
-        <v>1</v>
+      <c r="O3" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="P3" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="39" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" s="16" t="b">
+        <v>0</v>
       </c>
       <c r="S3" s="16" t="b">
         <v>0</v>
@@ -2196,8 +2214,8 @@
       <c r="T3" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="U3" s="16" t="b">
-        <v>0</v>
+      <c r="U3" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="V3" s="16" t="b">
         <v>0</v>
@@ -2235,38 +2253,47 @@
       <c r="AG3" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="AH3" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="3" t="b">
+      <c r="AH3" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="16" t="b">
         <v>0</v>
       </c>
       <c r="AK3" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="AM3" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="30" t="b">
+      <c r="AM3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="31" t="b">
         <v>0</v>
       </c>
       <c r="AQ3" s="30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:43" s="26" customFormat="1">
+      <c r="AR3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" s="26" customFormat="1">
       <c r="A4" s="29" t="s">
         <v>44</v>
       </c>
@@ -2309,13 +2336,13 @@
       <c r="N4" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="O4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="3" t="b">
+      <c r="O4" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" s="39" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="39" t="b">
         <v>1</v>
       </c>
       <c r="R4" s="3" t="b">
@@ -2370,34 +2397,43 @@
         <v>1</v>
       </c>
       <c r="AI4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ4" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK4" s="3" t="b">
         <v>1</v>
       </c>
       <c r="AL4" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM4" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN4" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO4" s="30" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="AM4" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="AP4" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ4" s="30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:43" s="26" customFormat="1">
+      <c r="AR4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" s="26" customFormat="1">
       <c r="A5" s="29" t="s">
         <v>45</v>
       </c>
@@ -2440,13 +2476,13 @@
       <c r="N5" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="O5" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="P5" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="16" t="b">
+      <c r="O5" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="P5" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="40" t="b">
         <v>0</v>
       </c>
       <c r="R5" s="16" t="b">
@@ -2512,23 +2548,32 @@
       <c r="AL5" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="AM5" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO5" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" s="26" customFormat="1">
+      <c r="AM5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" s="26" customFormat="1">
       <c r="A6" s="29" t="s">
         <v>46</v>
       </c>
@@ -2571,13 +2616,13 @@
       <c r="N6" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="O6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="3" t="b">
+      <c r="O6" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="40" t="b">
         <v>1</v>
       </c>
       <c r="R6" s="3" t="b">
@@ -2643,23 +2688,32 @@
       <c r="AL6" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="AM6" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN6" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="31" t="b">
-        <v>0</v>
+      <c r="AM6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="3" t="b">
+        <v>1</v>
       </c>
       <c r="AP6" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:43" s="16" customFormat="1">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:46" s="16" customFormat="1">
       <c r="A7" s="22" t="s">
         <v>47</v>
       </c>
@@ -2702,13 +2756,13 @@
       <c r="N7" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="O7" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="16" t="b">
+      <c r="O7" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="P7" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="40" t="b">
         <v>0</v>
       </c>
       <c r="R7" s="16" t="b">
@@ -2774,13 +2828,13 @@
       <c r="AL7" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="AM7" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="31" t="b">
+      <c r="AM7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="16" t="b">
         <v>0</v>
       </c>
       <c r="AP7" s="31" t="b">
@@ -2789,8 +2843,17 @@
       <c r="AQ7" s="31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:43" s="16" customFormat="1">
+      <c r="AR7" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
         <v>48</v>
       </c>
@@ -2833,13 +2896,13 @@
       <c r="N8" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="O8" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="P8" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="16" t="b">
+      <c r="O8" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="P8" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="40" t="b">
         <v>0</v>
       </c>
       <c r="R8" s="16" t="b">
@@ -2905,13 +2968,13 @@
       <c r="AL8" s="16" t="b">
         <v>0</v>
       </c>
-      <c r="AM8" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="31" t="b">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="31" t="b">
+      <c r="AM8" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="16" t="b">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="16" t="b">
         <v>0</v>
       </c>
       <c r="AP8" s="31" t="b">
@@ -2920,8 +2983,17 @@
       <c r="AQ8" s="31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:43" s="17" customFormat="1" ht="67.5">
+      <c r="AR8" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" s="17" customFormat="1" ht="67.5">
       <c r="A9" s="23" t="s">
         <v>49</v>
       </c>
@@ -2964,93 +3036,102 @@
       <c r="N9" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="O9" s="24" t="s">
+      <c r="O9" s="41" t="s">
+        <v>222</v>
+      </c>
+      <c r="P9" s="41" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q9" s="41" t="s">
+        <v>224</v>
+      </c>
+      <c r="R9" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="P9" s="24" t="s">
+      <c r="S9" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="Q9" s="24" t="s">
+      <c r="T9" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="R9" s="24" t="s">
+      <c r="U9" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="S9" s="24" t="s">
+      <c r="V9" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="T9" s="24" t="s">
+      <c r="W9" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="U9" s="24" t="s">
+      <c r="X9" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="V9" s="24" t="s">
+      <c r="Y9" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="W9" s="24" t="s">
+      <c r="Z9" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="X9" s="24" t="s">
+      <c r="AA9" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="Y9" s="24" t="s">
+      <c r="AB9" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="Z9" s="24" t="s">
+      <c r="AC9" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AA9" s="24" t="s">
+      <c r="AD9" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AB9" s="24" t="s">
+      <c r="AE9" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="AC9" s="24" t="s">
+      <c r="AF9" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="AD9" s="24" t="s">
+      <c r="AG9" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AE9" s="24" t="s">
+      <c r="AH9" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AF9" s="24" t="s">
+      <c r="AI9" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AG9" s="24" t="s">
+      <c r="AJ9" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AH9" s="24" t="s">
+      <c r="AK9" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AI9" s="24" t="s">
+      <c r="AL9" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="AJ9" s="24" t="s">
+      <c r="AM9" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="AK9" s="24" t="s">
+      <c r="AN9" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AL9" s="24" t="s">
+      <c r="AO9" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="AM9" s="32" t="s">
+      <c r="AP9" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="AN9" s="32" t="s">
+      <c r="AQ9" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="AO9" s="32" t="s">
+      <c r="AR9" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="AP9" s="33"/>
-      <c r="AQ9" s="33"/>
+      <c r="AS9" s="33"/>
+      <c r="AT9" s="33"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O3:Q3 AN5:AO6 S3:AG3 J3 AN7:AQ8 B7:AL8 B5:AM5 K6:N6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:T3 AQ5:AR6 V3:AJ3 J3 AQ7:AT8 K6:Q6 B5:AP5 B7:AO8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>

</xml_diff>

<commit_message>
new path for class's struct and ini files
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Player.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Player.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Component" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Record_Building!$E$1:$E$22</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -420,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="231">
   <si>
     <t>Id</t>
   </si>
@@ -1090,12 +1091,6 @@
     <t>PosY</t>
   </si>
   <si>
-    <t>PosZ</t>
-  </si>
-  <si>
-    <t>StateStartTime</t>
-  </si>
-  <si>
     <t>StateEndTime</t>
   </si>
   <si>
@@ -1148,6 +1143,15 @@
   </si>
   <si>
     <t>0job_level,1equipment,2static_BUFF,3runtime_BUFF,4Hero</t>
+  </si>
+  <si>
+    <t>Pos</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>vector3</t>
   </si>
 </sst>
 </file>
@@ -1845,7 +1849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
@@ -1905,16 +1909,16 @@
         <v>9</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M1" s="28" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="N1" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="O1" s="28" t="s">
         <v>158</v>
@@ -3025,25 +3029,25 @@
         <v>58</v>
       </c>
       <c r="K9" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="L9" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="M9" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="L9" s="41" t="s">
+      <c r="N9" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="M9" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="N9" s="41" t="s">
-        <v>224</v>
-      </c>
       <c r="O9" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="P9" s="41" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q9" s="41" t="s">
         <v>222</v>
-      </c>
-      <c r="P9" s="41" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q9" s="41" t="s">
-        <v>224</v>
       </c>
       <c r="R9" s="24" t="s">
         <v>60</v>
@@ -4282,7 +4286,7 @@
         <v>49</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
@@ -4440,7 +4444,7 @@
         <v>144</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>6</v>
@@ -4847,7 +4851,7 @@
         <v>49</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
@@ -5882,28 +5886,30 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="16.19921875" style="4" customWidth="1"/>
-    <col min="2" max="3" width="7.19921875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.19921875" style="4" customWidth="1"/>
     <col min="4" max="4" width="10.46484375" style="4" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="4" customWidth="1"/>
-    <col min="6" max="10" width="9" style="4"/>
-    <col min="11" max="11" width="12.6640625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="13.796875" style="4" customWidth="1"/>
-    <col min="13" max="13" width="9" style="4"/>
-    <col min="14" max="14" width="11.6640625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="13.796875" style="4" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="4"/>
+    <col min="6" max="6" width="13.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9" style="4"/>
+    <col min="9" max="9" width="12.6640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="13.796875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9" style="4"/>
+    <col min="12" max="12" width="11.6640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="13.796875" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5911,7 +5917,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1">
+    <row r="2" spans="1:6" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>141</v>
       </c>
@@ -5919,15 +5925,15 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1">
+    <row r="3" spans="1:6" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B3" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>43</v>
       </c>
@@ -5935,7 +5941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1">
+    <row r="5" spans="1:6" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
@@ -5943,7 +5949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1">
+    <row r="6" spans="1:6" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
@@ -5951,7 +5957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1">
+    <row r="7" spans="1:6" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
@@ -5959,7 +5965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1">
+    <row r="8" spans="1:6" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>192</v>
       </c>
@@ -5967,7 +5973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1">
+    <row r="9" spans="1:6" s="3" customFormat="1">
       <c r="A9" s="34" t="s">
         <v>205</v>
       </c>
@@ -5981,19 +5987,13 @@
         <v>208</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="F9" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="G9" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="3" customFormat="1">
+    </row>
+    <row r="10" spans="1:6" s="3" customFormat="1">
       <c r="A10" s="34" t="s">
         <v>40</v>
       </c>
@@ -6004,22 +6004,16 @@
         <v>41</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>41</v>
+        <v>229</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>41</v>
+        <v>230</v>
       </c>
       <c r="F10" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="3" customFormat="1">
+    </row>
+    <row r="11" spans="1:6" s="3" customFormat="1">
       <c r="A11" s="34" t="s">
         <v>49</v>
       </c>
@@ -6028,18 +6022,16 @@
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
       <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-    </row>
-    <row r="12" spans="1:8" s="2" customFormat="1">
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="3" customFormat="1">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>141</v>
       </c>
@@ -6047,15 +6039,15 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="3" customFormat="1">
+    <row r="14" spans="1:6" s="3" customFormat="1">
       <c r="A14" s="3" t="s">
         <v>142</v>
       </c>
       <c r="B14" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="3" customFormat="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -6063,7 +6055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="3" customFormat="1">
+    <row r="16" spans="1:6" s="3" customFormat="1">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -6071,7 +6063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="3" customFormat="1">
+    <row r="17" spans="1:6" s="3" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -6079,7 +6071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="3" customFormat="1">
+    <row r="18" spans="1:6" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
         <v>46</v>
       </c>
@@ -6087,7 +6079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="3" customFormat="1">
+    <row r="19" spans="1:6" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
         <v>48</v>
       </c>
@@ -6095,7 +6087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="3" customFormat="1">
+    <row r="20" spans="1:6" s="3" customFormat="1">
       <c r="A20" s="34" t="s">
         <v>205</v>
       </c>
@@ -6114,14 +6106,8 @@
       <c r="F20" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="G20" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="H20" s="34" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="3" customFormat="1">
+    </row>
+    <row r="21" spans="1:6" s="3" customFormat="1">
       <c r="A21" s="34" t="s">
         <v>40</v>
       </c>
@@ -6132,22 +6118,16 @@
         <v>41</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>41</v>
+        <v>229</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>41</v>
+        <v>229</v>
       </c>
       <c r="F21" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="3" customFormat="1">
+    </row>
+    <row r="22" spans="1:6" s="3" customFormat="1">
       <c r="A22" s="34" t="s">
         <v>49</v>
       </c>
@@ -6156,16 +6136,14 @@
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
       <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 E11:F11 B18 B19 I1:I1048576 G11:H19 D22:H1048576 A15:B17 E1:H8 D12:F19 A4:B5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6:B8 B18:B19 G1:G1048576 A15:B17 A4:B5 D12:D19 D22:D1048576 F1:F8 F11:F19 F22:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A9:B9 D9:F9 A20:B20 D20:F20 K40:K1048576"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:B10 D10:F10 A21:B21 D21:F21 K1:K39">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A9:B9 A20:B20 I40:I1048576 D20 D9"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:B10 A21:B21 I1:I39 D21 D10">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C21">
@@ -6201,10 +6179,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D1" t="s">
         <v>49</v>
@@ -6212,16 +6190,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>